<commit_message>
script updated for cleaning, and full composites done, need to clean names for weird spanish characters
</commit_message>
<xml_diff>
--- a/training_data/2007/basic_hitting.xlsx
+++ b/training_data/2007/basic_hitting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex_1/Desktop/MVP-Predictor/training_data/2007/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F0D2B0C-ECAC-1E44-B361-A1CDEB917B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434A99CB-FC96-294C-B804-B4490C3F7612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{20C4AF37-E108-6847-B20A-39B226BB0D68}"/>
+    <workbookView xWindow="3600" yWindow="3840" windowWidth="28040" windowHeight="17440" xr2:uid="{20C4AF37-E108-6847-B20A-39B226BB0D68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4022,8 +4022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33CCD70-62CF-454B-9F3E-2B76CE8F194F}">
   <dimension ref="A4:I1362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1343" workbookViewId="0">
-      <selection activeCell="B1363" sqref="B1363:I1363"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>